<commit_message>
Finished pipeline for news
</commit_message>
<xml_diff>
--- a/crawlers/results.xlsx
+++ b/crawlers/results.xlsx
@@ -472,20 +472,20 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>2.6</v>
+        <v>5.5</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -501,20 +501,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -565,14 +565,14 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -594,14 +594,14 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -617,20 +617,20 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>11</v>
-      </c>
       <c r="E7" t="n">
-        <v>2.1</v>
+        <v>4.1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -652,14 +652,14 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>1.9</v>
+        <v>1.1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3</v>
+        <v>3.1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -704,25 +704,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4</v>
+        <v>1.1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -733,20 +733,20 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -762,20 +762,20 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>1.8</v>
+        <v>5.3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -791,25 +791,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.3999999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -820,20 +820,20 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>2.2</v>
+        <v>6.2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -849,25 +849,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7000000000000001</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -878,10 +878,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
         <v>6</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -907,20 +907,20 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>3.1</v>
+        <v>5.6</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -942,14 +942,14 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -971,19 +971,19 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
-        <v>2.6</v>
+        <v>0.8</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>rising</t>
+          <t>stable</t>
         </is>
       </c>
     </row>
@@ -994,20 +994,20 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -1032,16 +1032,16 @@
         <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>rising</t>
+          <t>stable</t>
         </is>
       </c>
     </row>
@@ -1052,25 +1052,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9</v>
+        <v>2.5</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -1081,25 +1081,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3</v>
+        <v>1.1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2023-05-07 19:14:21</t>
+          <t>2023-05-08 17:24:02</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Init Realtime prices tab
</commit_message>
<xml_diff>
--- a/crawlers/results.xlsx
+++ b/crawlers/results.xlsx
@@ -497,25 +497,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.8</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -526,20 +526,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>4.2</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>falling</t>
         </is>
       </c>
     </row>
@@ -584,25 +584,25 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>3.7</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -613,25 +613,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -642,20 +642,20 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>1.2</v>
+        <v>7.8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -671,20 +671,20 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>5.2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -700,25 +700,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -729,25 +729,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -758,20 +758,20 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E11" t="n">
-        <v>4.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -787,20 +787,20 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E12" t="n">
-        <v>2.1</v>
+        <v>13.5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -816,20 +816,20 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E13" t="n">
-        <v>1.2</v>
+        <v>11.8</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -845,20 +845,20 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E14" t="n">
-        <v>2.1</v>
+        <v>15.6</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -874,25 +874,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>-1</v>
+        <v>3.7</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -903,20 +903,20 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E16" t="n">
-        <v>4.1</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -932,20 +932,20 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E17" t="n">
-        <v>0.09999999999999998</v>
+        <v>4.4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -961,25 +961,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -990,20 +990,20 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E19" t="n">
-        <v>2.4</v>
+        <v>14.4</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1019,25 +1019,25 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2</v>
+        <v>-0.1000000000000001</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>falling</t>
         </is>
       </c>
     </row>
@@ -1048,20 +1048,20 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E21" t="n">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1077,25 +1077,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>
@@ -1106,25 +1106,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2023-05-16 14:14:29</t>
+          <t>2023-05-17 17:50:07</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>stable</t>
+          <t>rising</t>
         </is>
       </c>
     </row>

</xml_diff>